<commit_message>
Update finding for alleviation and exacerbation.xlsx
</commit_message>
<xml_diff>
--- a/Final Project/finding for alleviation and exacerbation.xlsx
+++ b/Final Project/finding for alleviation and exacerbation.xlsx
@@ -14,9 +14,151 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>exacerbate</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+  <si>
+    <t>%(n)of students who think exacerbation
+N = 1179</t>
+  </si>
+  <si>
+    <t>idep.diff.know.students</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difficulty getting to know other students in class </t>
+  </si>
+  <si>
+    <t>61.74% (728)</t>
+  </si>
+  <si>
+    <t>idep.diff.help.students</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difficulty getting help from other students in class </t>
+  </si>
+  <si>
+    <t>49.53% (584)</t>
+  </si>
+  <si>
+    <t>idep.talk.unknown</t>
+  </si>
+  <si>
+    <t>Needing to talk with students who I don’t know during online group work</t>
+  </si>
+  <si>
+    <t>43.60% (514)</t>
+  </si>
+  <si>
+    <t>idep.diff.know.instructor</t>
+  </si>
+  <si>
+    <t>Difficulty getting to know instructors</t>
+  </si>
+  <si>
+    <t>51.31% (605)</t>
+  </si>
+  <si>
+    <t>idep.diff.help.instructor</t>
+  </si>
+  <si>
+    <t>Difficulty getting help from instructors</t>
+  </si>
+  <si>
+    <t>47.41% (559)</t>
+  </si>
+  <si>
+    <t>idep.compare</t>
+  </si>
+  <si>
+    <t>Comparing myself to other students</t>
+  </si>
+  <si>
+    <t>45.89% (541)</t>
+  </si>
+  <si>
+    <t>idep.not.inperson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not having to show up in person to online science courses </t>
+  </si>
+  <si>
+    <t>30.28% (357)</t>
+  </si>
+  <si>
+    <t>idep.pace</t>
+  </si>
+  <si>
+    <t>Deciding the pace at which I work through an online science course</t>
+  </si>
+  <si>
+    <t>27.48% (324)</t>
+  </si>
+  <si>
+    <t>idep.camera</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Being on camera</t>
+  </si>
+  <si>
+    <t>39.27% (463)</t>
+  </si>
+  <si>
+    <t>idep.nav.tech</t>
+  </si>
+  <si>
+    <t>Needing to navigate technology in high-pressure situations (e.g., during exams)</t>
+  </si>
+  <si>
+    <t>45.29% (534</t>
+  </si>
+  <si>
+    <t>idep.proctor.exam</t>
+  </si>
+  <si>
+    <t>Online monitored proctored testing</t>
+  </si>
+  <si>
+    <t>57.51% (678)</t>
+  </si>
+  <si>
+    <t>idep.questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Struggling to have questions answered </t>
+  </si>
+  <si>
+    <t>48.43% (571)</t>
+  </si>
+  <si>
+    <t>idep.comm.instructor</t>
+  </si>
+  <si>
+    <t>Struggling to communicate effectively with the instructor</t>
+  </si>
+  <si>
+    <t>46.73% (551)</t>
+  </si>
+  <si>
+    <t>idep.home.distract</t>
+  </si>
+  <si>
+    <t>At-home distractions that can interfere with online science courses</t>
+  </si>
+  <si>
+    <t>54.37% (641)</t>
+  </si>
+  <si>
+    <t>idep.personal.tech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The potential for personal technology issues (e.g., unstable internet connection) </t>
+  </si>
+  <si>
+    <t>43.94% (518)</t>
+  </si>
+  <si>
+    <t>idep.other</t>
+  </si>
+  <si>
+    <t>idep.nothing</t>
   </si>
 </sst>
 </file>
@@ -29,13 +171,19 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -490,10 +638,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -502,34 +650,31 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -541,100 +686,115 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -955,21 +1115,203 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="52.125" customWidth="1"/>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="60.375" customWidth="1"/>
+    <col min="3" max="3" width="23.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" ht="40.5" spans="2:3">
+      <c r="B1" s="1"/>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
+    </row>
+    <row r="2" ht="15.75" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
generate alleviate and exacerbate files
</commit_message>
<xml_diff>
--- a/Final Project/finding for alleviation and exacerbation.xlsx
+++ b/Final Project/finding for alleviation and exacerbation.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="exacerbate" sheetId="1" r:id="rId1"/>
+    <sheet name="alleviate" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
   <si>
     <t>%(n)of students who think exacerbation
 N = 1179</t>
@@ -155,10 +156,142 @@
     <t>43.94% (518)</t>
   </si>
   <si>
-    <t>idep.other</t>
-  </si>
-  <si>
-    <t>idep.nothing</t>
+    <t>ddep.easy.know.students</t>
+  </si>
+  <si>
+    <t>Easily getting to know other students in class</t>
+  </si>
+  <si>
+    <t>24.68% (291)</t>
+  </si>
+  <si>
+    <t>ddep.easy.help.students</t>
+  </si>
+  <si>
+    <t>Easily getting help from other students in class</t>
+  </si>
+  <si>
+    <t>ddep.easy.know.instructor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Easily getting to know instructors </t>
+  </si>
+  <si>
+    <t>24.51% (289)</t>
+  </si>
+  <si>
+    <t>ddep.easy.help.instructor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Easily getting help from instructors</t>
+  </si>
+  <si>
+    <t>31.21% (368)</t>
+  </si>
+  <si>
+    <t>ddep.instr.cares</t>
+  </si>
+  <si>
+    <t>Having an instructor who appears to care about mental health</t>
+  </si>
+  <si>
+    <t>58.18% (686)</t>
+  </si>
+  <si>
+    <t>ddep.flex.when</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The flexibility of doing coursework </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> I want</t>
+    </r>
+  </si>
+  <si>
+    <t>65.06% (767)</t>
+  </si>
+  <si>
+    <t>ddep.flex.where</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The flexibility of doing coursework </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>where</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> I want </t>
+    </r>
+  </si>
+  <si>
+    <t>63.95% (754)</t>
+  </si>
+  <si>
+    <t>ddep.not.seen</t>
+  </si>
+  <si>
+    <t>Being able to engage in an online science course without having to be seen</t>
+  </si>
+  <si>
+    <t>47.84% (114)</t>
+  </si>
+  <si>
+    <t>ddep.answer.qs</t>
+  </si>
+  <si>
+    <t>Getting questions answered</t>
+  </si>
+  <si>
+    <t>33.67% (397)</t>
+  </si>
+  <si>
+    <t>ddep.clear.comm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear communication with instructors </t>
+  </si>
+  <si>
+    <t>37.40% (441)</t>
+  </si>
+  <si>
+    <t>ddep.anonymous</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Being anonymous or being able to share my opinion without it being associated with my face</t>
+  </si>
+  <si>
+    <t>45.29% (534)</t>
   </si>
 </sst>
 </file>
@@ -168,10 +301,10 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,6 +461,13 @@
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="33">
@@ -647,16 +787,16 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -787,10 +927,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1118,7 +1258,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
@@ -1129,189 +1269,333 @@
   </cols>
   <sheetData>
     <row r="1" ht="40.5" spans="2:3">
-      <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" ht="15.75" spans="1:3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" ht="15.75" spans="1:3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" ht="15.75" spans="1:3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="1:3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="1:3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="1:3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" ht="15.75" spans="1:3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="1:3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" ht="15.75" spans="1:3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" ht="15.75" spans="1:3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="70.75" customWidth="1"/>
+    <col min="3" max="3" width="24.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="40.5" spans="3:3">
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" spans="1:3">
+      <c r="A2" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" spans="1:3">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" spans="1:3">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" spans="1:3">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" spans="1:3">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" spans="1:3">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" spans="1:3">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" spans="1:3">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" spans="1:3">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" spans="1:3">
+      <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" spans="1:3">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>